<commit_message>
Add type and cover in sheet and adjust template
</commit_message>
<xml_diff>
--- a/consumers.xlsx
+++ b/consumers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -37,6 +37,12 @@
     <t xml:space="preserve">Consumo(kWh)</t>
   </si>
   <si>
+    <t xml:space="preserve">Tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobertura(%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fischer, Livingston and Smith</t>
   </si>
   <si>
@@ -49,6 +55,9 @@
     <t xml:space="preserve">Shoals</t>
   </si>
   <si>
+    <t xml:space="preserve">Residencial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tapia, Patel and Richardson</t>
   </si>
   <si>
@@ -61,6 +70,9 @@
     <t xml:space="preserve">Heights</t>
   </si>
   <si>
+    <t xml:space="preserve">Comercial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Solomon-Molina</t>
   </si>
   <si>
@@ -85,6 +97,9 @@
     <t xml:space="preserve">Fords</t>
   </si>
   <si>
+    <t xml:space="preserve">Industrial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frye, Jones and Edwards</t>
   </si>
   <si>
@@ -215,63 +230,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gateway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cantu, Morris and Williams</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2455844871084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Danieltown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torres LLC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3611278772390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Jared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parsons, Campos and Casey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8567003654453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wintersville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brooks-Wagner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8543418605808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lake Melindahaven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norton-Vargas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2672006205888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sherrymouth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranch</t>
   </si>
 </sst>
 </file>
@@ -362,13 +320,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -388,22 +354,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,25 +387,37 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>407</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,39 +425,51 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>9667</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>1046</v>
+        <v>10046</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,341 +477,331 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>603</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>5095</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15095</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>7032</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>6146</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13012</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>3544</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35440</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>410</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>2298</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22980</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>772</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>4104</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>4319</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>3668</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>7147</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>5505</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>4587</v>
-      </c>
-    </row>
+        <v>16760</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add distributor tax and run migrations
</commit_message>
<xml_diff>
--- a/consumers.xlsx
+++ b/consumers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cobertura(%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarifa da Distribuidora</t>
   </si>
   <si>
     <t xml:space="preserve">Fischer, Livingston and Smith</t>
@@ -354,10 +357,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,6 +372,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,31 +397,37 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>407</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1.12307169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,25 +435,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>9667</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1.04820025</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,25 +464,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10046</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>95</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>1.12307169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,25 +493,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>603</v>
+        <v>1186</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,25 +522,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>15095</v>
+        <v>16633</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>95</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1.04820025</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,25 +551,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>7032</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1.04820025</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,25 +580,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>6146</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,25 +609,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>13012</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>95</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,25 +638,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>35440</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>99</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1.12307169</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,25 +667,28 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>410</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,25 +696,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>22980</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>99</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,25 +725,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>772</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1.04820025</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,25 +754,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>4104</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.95871974</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,25 +783,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>4319</v>
+        <v>1051</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>90</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1.12307169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,25 +812,28 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>16760</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>95</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1.12307169</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Remove some consumers from sheet
</commit_message>
<xml_diff>
--- a/consumers.xlsx
+++ b/consumers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -173,66 +173,6 @@
   </si>
   <si>
     <t xml:space="preserve">Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taylor LLC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5919790649113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Matthew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skyway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hardin-Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6672053353255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Julia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wright Inc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3067064730530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Robertberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flores-Bishop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5661901620138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lake Susan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ford</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenkins and Sons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0840094828773</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeremymouth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gateway</t>
   </si>
 </sst>
 </file>
@@ -359,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -692,149 +632,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>22980</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>99</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>0.95871974</v>
-      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>772</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>1.04820025</v>
-      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>4104</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>0.95871974</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>1051</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>1.12307169</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>16760</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>1.12307169</v>
-      </c>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="3"/>

</xml_diff>